<commit_message>
texto final confianza en instituciones
</commit_message>
<xml_diff>
--- a/data/latino/confianzas2020.xlsx
+++ b/data/latino/confianzas2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Trabajo\UMAD\Piso I\Piso-I-OP\data\latino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC02ED15-2964-4994-9B70-0EDA6AA3619E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534FB546-EF17-4F30-93BF-183A0FBE85BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,9 +73,6 @@
     <t xml:space="preserve"> Uruguay</t>
   </si>
   <si>
-    <t xml:space="preserve"> Venezuela_x000D_</t>
-  </si>
-  <si>
     <t>Mucha</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>Total América Latina</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Venezuela</t>
   </si>
 </sst>
 </file>
@@ -182,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -215,6 +215,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,8 +587,8 @@
   <dimension ref="A1:AA151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B133" sqref="B133"/>
+      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -598,22 +601,22 @@
   <sheetData>
     <row r="1" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -638,10 +641,10 @@
     </row>
     <row r="2" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="4">
         <v>0.14499999999999999</v>
@@ -678,7 +681,7 @@
     </row>
     <row r="3" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -718,7 +721,7 @@
     </row>
     <row r="4" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -758,7 +761,7 @@
     </row>
     <row r="5" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
@@ -798,7 +801,7 @@
     </row>
     <row r="6" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
@@ -818,7 +821,7 @@
     </row>
     <row r="7" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
@@ -838,7 +841,7 @@
     </row>
     <row r="8" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
@@ -858,7 +861,7 @@
     </row>
     <row r="9" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
@@ -878,7 +881,7 @@
     </row>
     <row r="10" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
@@ -898,7 +901,7 @@
     </row>
     <row r="11" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
@@ -918,7 +921,7 @@
     </row>
     <row r="12" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>9</v>
@@ -938,7 +941,7 @@
     </row>
     <row r="13" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>10</v>
@@ -958,7 +961,7 @@
     </row>
     <row r="14" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>11</v>
@@ -978,7 +981,7 @@
     </row>
     <row r="15" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>12</v>
@@ -998,7 +1001,7 @@
     </row>
     <row r="16" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>13</v>
@@ -1018,7 +1021,7 @@
     </row>
     <row r="17" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>14</v>
@@ -1038,7 +1041,7 @@
     </row>
     <row r="18" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>15</v>
@@ -1058,9 +1061,9 @@
     </row>
     <row r="19" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="4">
@@ -1078,10 +1081,10 @@
     </row>
     <row r="20" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="C20" s="4">
         <v>0.11599999999999999</v>
@@ -1098,10 +1101,10 @@
     </row>
     <row r="21" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="4">
         <v>0.38200000000000001</v>
@@ -1118,7 +1121,7 @@
     </row>
     <row r="22" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>0</v>
@@ -1138,7 +1141,7 @@
     </row>
     <row r="23" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>1</v>
@@ -1158,7 +1161,7 @@
     </row>
     <row r="24" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>2</v>
@@ -1178,7 +1181,7 @@
     </row>
     <row r="25" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>3</v>
@@ -1198,7 +1201,7 @@
     </row>
     <row r="26" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>4</v>
@@ -1218,7 +1221,7 @@
     </row>
     <row r="27" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
@@ -1238,7 +1241,7 @@
     </row>
     <row r="28" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>6</v>
@@ -1258,7 +1261,7 @@
     </row>
     <row r="29" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>7</v>
@@ -1298,7 +1301,7 @@
     </row>
     <row r="30" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>8</v>
@@ -1338,7 +1341,7 @@
     </row>
     <row r="31" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>9</v>
@@ -1378,7 +1381,7 @@
     </row>
     <row r="32" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>10</v>
@@ -1418,7 +1421,7 @@
     </row>
     <row r="33" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>11</v>
@@ -1458,7 +1461,7 @@
     </row>
     <row r="34" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>12</v>
@@ -1478,7 +1481,7 @@
     </row>
     <row r="35" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>13</v>
@@ -1498,7 +1501,7 @@
     </row>
     <row r="36" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>14</v>
@@ -1518,7 +1521,7 @@
     </row>
     <row r="37" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>15</v>
@@ -1538,7 +1541,7 @@
     </row>
     <row r="38" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>16</v>
@@ -1558,10 +1561,10 @@
     </row>
     <row r="39" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C39" s="4">
         <v>0.47899999999999998</v>
@@ -1578,10 +1581,10 @@
     </row>
     <row r="40" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40" s="7">
         <v>0.11800000000000001</v>
@@ -1598,7 +1601,7 @@
     </row>
     <row r="41" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>0</v>
@@ -1618,7 +1621,7 @@
     </row>
     <row r="42" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>1</v>
@@ -1638,7 +1641,7 @@
     </row>
     <row r="43" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>2</v>
@@ -1658,7 +1661,7 @@
     </row>
     <row r="44" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>3</v>
@@ -1678,7 +1681,7 @@
     </row>
     <row r="45" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>4</v>
@@ -1698,7 +1701,7 @@
     </row>
     <row r="46" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>5</v>
@@ -1718,7 +1721,7 @@
     </row>
     <row r="47" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>6</v>
@@ -1738,7 +1741,7 @@
     </row>
     <row r="48" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>7</v>
@@ -1758,7 +1761,7 @@
     </row>
     <row r="49" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>8</v>
@@ -1778,7 +1781,7 @@
     </row>
     <row r="50" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>9</v>
@@ -1798,7 +1801,7 @@
     </row>
     <row r="51" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>10</v>
@@ -1818,7 +1821,7 @@
     </row>
     <row r="52" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>11</v>
@@ -1838,7 +1841,7 @@
     </row>
     <row r="53" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>12</v>
@@ -1878,7 +1881,7 @@
     </row>
     <row r="54" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>13</v>
@@ -1918,7 +1921,7 @@
     </row>
     <row r="55" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>14</v>
@@ -1958,7 +1961,7 @@
     </row>
     <row r="56" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>15</v>
@@ -1998,7 +2001,7 @@
     </row>
     <row r="57" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>16</v>
@@ -2038,10 +2041,10 @@
     </row>
     <row r="58" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C58" s="7">
         <v>3.7000000000000005E-2</v>
@@ -2058,10 +2061,10 @@
     </row>
     <row r="59" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C59" s="10">
         <v>0.183</v>
@@ -2078,7 +2081,7 @@
     </row>
     <row r="60" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>0</v>
@@ -2098,7 +2101,7 @@
     </row>
     <row r="61" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>1</v>
@@ -2118,7 +2121,7 @@
     </row>
     <row r="62" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>2</v>
@@ -2138,7 +2141,7 @@
     </row>
     <row r="63" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>3</v>
@@ -2158,7 +2161,7 @@
     </row>
     <row r="64" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>4</v>
@@ -2178,7 +2181,7 @@
     </row>
     <row r="65" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>6</v>
@@ -2198,7 +2201,7 @@
     </row>
     <row r="66" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>7</v>
@@ -2218,7 +2221,7 @@
     </row>
     <row r="67" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>8</v>
@@ -2238,7 +2241,7 @@
     </row>
     <row r="68" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>9</v>
@@ -2258,7 +2261,7 @@
     </row>
     <row r="69" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>10</v>
@@ -2278,7 +2281,7 @@
     </row>
     <row r="70" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>11</v>
@@ -2298,7 +2301,7 @@
     </row>
     <row r="71" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>12</v>
@@ -2318,7 +2321,7 @@
     </row>
     <row r="72" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>14</v>
@@ -2338,7 +2341,7 @@
     </row>
     <row r="73" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>15</v>
@@ -2358,7 +2361,7 @@
     </row>
     <row r="74" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>16</v>
@@ -2378,10 +2381,10 @@
     </row>
     <row r="75" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C75" s="10">
         <v>8.5000000000000006E-2</v>
@@ -2398,10 +2401,10 @@
     </row>
     <row r="76" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C76" s="10">
         <v>0.03</v>
@@ -2418,7 +2421,7 @@
     </row>
     <row r="77" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>0</v>
@@ -2438,7 +2441,7 @@
     </row>
     <row r="78" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>1</v>
@@ -2478,7 +2481,7 @@
     </row>
     <row r="79" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>2</v>
@@ -2518,7 +2521,7 @@
     </row>
     <row r="80" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>3</v>
@@ -2558,7 +2561,7 @@
     </row>
     <row r="81" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>4</v>
@@ -2598,7 +2601,7 @@
     </row>
     <row r="82" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>5</v>
@@ -2638,7 +2641,7 @@
     </row>
     <row r="83" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>6</v>
@@ -2658,7 +2661,7 @@
     </row>
     <row r="84" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>7</v>
@@ -2678,7 +2681,7 @@
     </row>
     <row r="85" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>8</v>
@@ -2698,7 +2701,7 @@
     </row>
     <row r="86" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>9</v>
@@ -2718,7 +2721,7 @@
     </row>
     <row r="87" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>10</v>
@@ -2738,7 +2741,7 @@
     </row>
     <row r="88" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>11</v>
@@ -2758,7 +2761,7 @@
     </row>
     <row r="89" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>12</v>
@@ -2778,7 +2781,7 @@
     </row>
     <row r="90" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>13</v>
@@ -2798,7 +2801,7 @@
     </row>
     <row r="91" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>14</v>
@@ -2818,7 +2821,7 @@
     </row>
     <row r="92" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>15</v>
@@ -2838,7 +2841,7 @@
     </row>
     <row r="93" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>16</v>
@@ -2858,10 +2861,10 @@
     </row>
     <row r="94" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C94" s="10">
         <v>3.3000000000000002E-2</v>
@@ -2878,10 +2881,10 @@
     </row>
     <row r="95" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B95" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C95" s="12">
         <v>0.106</v>
@@ -2898,7 +2901,7 @@
     </row>
     <row r="96" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B96" s="11" t="s">
         <v>0</v>
@@ -2918,7 +2921,7 @@
     </row>
     <row r="97" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B97" s="11" t="s">
         <v>1</v>
@@ -2938,7 +2941,7 @@
     </row>
     <row r="98" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B98" s="11" t="s">
         <v>2</v>
@@ -2958,7 +2961,7 @@
     </row>
     <row r="99" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B99" s="11" t="s">
         <v>3</v>
@@ -2978,7 +2981,7 @@
     </row>
     <row r="100" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B100" s="11" t="s">
         <v>4</v>
@@ -2998,7 +3001,7 @@
     </row>
     <row r="101" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B101" s="11" t="s">
         <v>5</v>
@@ -3018,7 +3021,7 @@
     </row>
     <row r="102" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B102" s="11" t="s">
         <v>6</v>
@@ -3038,7 +3041,7 @@
     </row>
     <row r="103" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B103" s="11" t="s">
         <v>7</v>
@@ -3058,7 +3061,7 @@
     </row>
     <row r="104" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B104" s="11" t="s">
         <v>8</v>
@@ -3078,7 +3081,7 @@
     </row>
     <row r="105" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B105" s="11" t="s">
         <v>9</v>
@@ -3118,7 +3121,7 @@
     </row>
     <row r="106" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B106" s="11" t="s">
         <v>10</v>
@@ -3158,7 +3161,7 @@
     </row>
     <row r="107" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B107" s="11" t="s">
         <v>11</v>
@@ -3198,7 +3201,7 @@
     </row>
     <row r="108" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B108" s="11" t="s">
         <v>12</v>
@@ -3238,7 +3241,7 @@
     </row>
     <row r="109" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B109" s="11" t="s">
         <v>13</v>
@@ -3278,7 +3281,7 @@
     </row>
     <row r="110" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B110" s="11" t="s">
         <v>14</v>
@@ -3298,7 +3301,7 @@
     </row>
     <row r="111" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B111" s="11" t="s">
         <v>15</v>
@@ -3318,7 +3321,7 @@
     </row>
     <row r="112" spans="1:26" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B112" s="11" t="s">
         <v>16</v>
@@ -3338,10 +3341,10 @@
     </row>
     <row r="113" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C113" s="12">
         <v>8.4000000000000005E-2</v>
@@ -3378,10 +3381,10 @@
     </row>
     <row r="114" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C114" s="14">
         <v>7.0000000000000007E-2</v>
@@ -3418,7 +3421,7 @@
     </row>
     <row r="115" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B115" s="13" t="s">
         <v>0</v>
@@ -3458,7 +3461,7 @@
     </row>
     <row r="116" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B116" s="13" t="s">
         <v>1</v>
@@ -3498,7 +3501,7 @@
     </row>
     <row r="117" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B117" s="13" t="s">
         <v>2</v>
@@ -3538,7 +3541,7 @@
     </row>
     <row r="118" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B118" s="13" t="s">
         <v>3</v>
@@ -3558,7 +3561,7 @@
     </row>
     <row r="119" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B119" s="13" t="s">
         <v>4</v>
@@ -3578,7 +3581,7 @@
     </row>
     <row r="120" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B120" s="13" t="s">
         <v>5</v>
@@ -3598,7 +3601,7 @@
     </row>
     <row r="121" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B121" s="13" t="s">
         <v>6</v>
@@ -3618,7 +3621,7 @@
     </row>
     <row r="122" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B122" s="13" t="s">
         <v>7</v>
@@ -3638,7 +3641,7 @@
     </row>
     <row r="123" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B123" s="13" t="s">
         <v>8</v>
@@ -3658,7 +3661,7 @@
     </row>
     <row r="124" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B124" s="13" t="s">
         <v>9</v>
@@ -3678,7 +3681,7 @@
     </row>
     <row r="125" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B125" s="13" t="s">
         <v>10</v>
@@ -3698,7 +3701,7 @@
     </row>
     <row r="126" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B126" s="13" t="s">
         <v>11</v>
@@ -3718,7 +3721,7 @@
     </row>
     <row r="127" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B127" s="13" t="s">
         <v>12</v>
@@ -3738,7 +3741,7 @@
     </row>
     <row r="128" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B128" s="13" t="s">
         <v>13</v>
@@ -3758,7 +3761,7 @@
     </row>
     <row r="129" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B129" s="13" t="s">
         <v>14</v>
@@ -3778,7 +3781,7 @@
     </row>
     <row r="130" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B130" s="13" t="s">
         <v>15</v>
@@ -3798,7 +3801,7 @@
     </row>
     <row r="131" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B131" s="13" t="s">
         <v>16</v>
@@ -3818,10 +3821,10 @@
     </row>
     <row r="132" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B132" s="13" t="s">
-        <v>17</v>
+        <v>27</v>
+      </c>
+      <c r="B132" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="C132" s="14">
         <v>5.7999999999999996E-2</v>
@@ -3838,10 +3841,10 @@
     </row>
     <row r="133" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B133" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C133" s="16">
         <v>5.2000000000000005E-2</v>
@@ -3858,7 +3861,7 @@
     </row>
     <row r="134" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B134" s="15" t="s">
         <v>0</v>
@@ -3878,7 +3881,7 @@
     </row>
     <row r="135" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B135" s="15" t="s">
         <v>1</v>
@@ -3898,7 +3901,7 @@
     </row>
     <row r="136" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B136" s="15" t="s">
         <v>2</v>
@@ -3918,7 +3921,7 @@
     </row>
     <row r="137" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B137" s="15" t="s">
         <v>3</v>
@@ -3938,7 +3941,7 @@
     </row>
     <row r="138" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B138" s="15" t="s">
         <v>4</v>
@@ -3958,7 +3961,7 @@
     </row>
     <row r="139" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B139" s="15" t="s">
         <v>5</v>
@@ -3978,7 +3981,7 @@
     </row>
     <row r="140" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B140" s="15" t="s">
         <v>6</v>
@@ -3998,7 +4001,7 @@
     </row>
     <row r="141" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B141" s="15" t="s">
         <v>7</v>
@@ -4018,7 +4021,7 @@
     </row>
     <row r="142" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B142" s="15" t="s">
         <v>8</v>
@@ -4038,7 +4041,7 @@
     </row>
     <row r="143" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B143" s="15" t="s">
         <v>9</v>
@@ -4058,7 +4061,7 @@
     </row>
     <row r="144" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B144" s="15" t="s">
         <v>10</v>
@@ -4078,7 +4081,7 @@
     </row>
     <row r="145" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B145" s="15" t="s">
         <v>11</v>
@@ -4098,7 +4101,7 @@
     </row>
     <row r="146" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B146" s="15" t="s">
         <v>12</v>
@@ -4118,7 +4121,7 @@
     </row>
     <row r="147" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B147" s="15" t="s">
         <v>13</v>
@@ -4138,7 +4141,7 @@
     </row>
     <row r="148" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B148" s="15" t="s">
         <v>14</v>
@@ -4158,7 +4161,7 @@
     </row>
     <row r="149" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B149" s="15" t="s">
         <v>15</v>
@@ -4178,7 +4181,7 @@
     </row>
     <row r="150" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B150" s="15" t="s">
         <v>16</v>
@@ -4198,10 +4201,10 @@
     </row>
     <row r="151" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B151" s="15" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C151" s="16">
         <v>6.3E-2</v>

</xml_diff>